<commit_message>
Adapt to changed format of excel file
</commit_message>
<xml_diff>
--- a/barclaycard2homebank/testfiles/Umsaetze.xlsx
+++ b/barclaycard2homebank/testfiles/Umsaetze.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
   <si>
     <t xml:space="preserve">Transaktionsansicht</t>
   </si>
@@ -76,13 +76,10 @@
     <t xml:space="preserve">Referenznummer</t>
   </si>
   <si>
-    <t xml:space="preserve">Transaktionsdatum</t>
-  </si>
-  <si>
     <t xml:space="preserve">Buchungsdatum</t>
   </si>
   <si>
-    <t xml:space="preserve">Betrag in EUR</t>
+    <t xml:space="preserve">Betrag</t>
   </si>
   <si>
     <t xml:space="preserve">Beschreibung</t>
@@ -97,7 +94,7 @@
     <t xml:space="preserve">Originalbetrag</t>
   </si>
   <si>
-    <t xml:space="preserve">Mögliche Ratenkäufe</t>
+    <t xml:space="preserve">Mögliche Zahlpläne</t>
   </si>
   <si>
     <t xml:space="preserve">Land</t>
@@ -412,7 +409,7 @@
   <dimension ref="A2:N19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -500,7 +497,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -508,308 +505,308 @@
         <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="I14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="L14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="M14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="N14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="F15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="I15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M15" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="N15" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="F16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="I16" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="L16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M16" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="N16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="F17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="I17" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="L17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M17" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="N17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="K18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M18" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="N18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="F19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="I19" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="M19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M19" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="N19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>